<commit_message>
English Language Table Data
</commit_message>
<xml_diff>
--- a/Language Data/Data.xlsx
+++ b/Language Data/Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\53276\OneDrive\Documents\MathsProject\Language Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{784BABF8-4034-4701-859F-BE4DC9E512C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C4E0EFF-25C9-4A40-A8D0-687BD5E870DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{CCE9E3C6-6CED-41B5-BE3F-22AB5F066C30}"/>
   </bookViews>
@@ -2774,10 +2774,191 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>56684</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>9262</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C6CB7FF-E4B2-74A1-F4C6-E33A6D42911C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7972425" y="0"/>
+          <a:ext cx="3723809" cy="2104762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>599609</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>8738</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{969BEBA3-A6C7-8287-E4F2-5919C18FE207}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4248150" y="0"/>
+          <a:ext cx="3723809" cy="6295238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>599609</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>56363</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{652EE053-62FB-6B73-BD1F-88A473CCD180}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4248150" y="6334125"/>
+          <a:ext cx="3723809" cy="6295238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>609134</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>46814</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{809DCDE7-ED80-B9D2-55B5-F1F9465CED87}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4257675" y="12801600"/>
+          <a:ext cx="3723809" cy="6485714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7E917053-E9CE-4742-AA29-FFC184437467}" name="Table1" displayName="Table1" ref="A1:H100">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H100">
-    <sortCondition ref="B1:B100"/>
+    <sortCondition ref="A1:A100"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{56C0FDDF-B280-41BC-91E9-7D29EABE3154}" name="Vertex" totalsRowLabel="Total"/>
@@ -10838,7 +11019,7 @@
   <dimension ref="A1:H100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R9" sqref="R9"/>
+      <selection activeCell="T28" sqref="T28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13452,8 +13633,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>